<commit_message>
some small inconsquential changes
</commit_message>
<xml_diff>
--- a/wildwood-xlsx-data/survey1.xlsx
+++ b/wildwood-xlsx-data/survey1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kswan\Desktop\Year 3 Semester 1\Artificial Intelligence\AI course programming\Projects\project 2\wildwood-csv-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kswan\Desktop\Year 3 Semester 1\Artificial Intelligence\AI course programming\Projects\project 2\wildwood-xlsx-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA60B55-11E7-48CE-B09A-99316252E28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FC7D38-90D0-475B-8BE0-D9A5AEE92D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey1" sheetId="1" r:id="rId1"/>
@@ -559,7 +559,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1393,14 +1393,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DE110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="CC1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="28.1796875" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" customWidth="1"/>
+    <col min="7" max="7" width="25.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" customWidth="1"/>
+    <col min="9" max="9" width="41.26953125" customWidth="1"/>
+    <col min="31" max="31" width="23.1796875" customWidth="1"/>
+    <col min="36" max="36" width="33" customWidth="1"/>
+    <col min="51" max="51" width="26.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:109" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>